<commit_message>
Introducing bar codes for "codice fiscale"
</commit_message>
<xml_diff>
--- a/tables/xls/it/70_Volontari attesi.xlsx
+++ b/tables/xls/it/70_Volontari attesi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>PROVINCIA</t>
   </si>
@@ -48,6 +48,15 @@
     <t>AUTISTA</t>
   </si>
   <si>
+    <t>PRANZO</t>
+  </si>
+  <si>
+    <t>CENA</t>
+  </si>
+  <si>
+    <t>BENEFICI DI LEGGE</t>
+  </si>
+  <si>
     <t>DATA ARRIVO</t>
   </si>
   <si>
@@ -63,9 +72,6 @@
     <t>TURNO</t>
   </si>
   <si>
-    <t>PROBLEMI ALIMENTARI</t>
-  </si>
-  <si>
     <t>CODICE ORGANIZZAZIONE</t>
   </si>
   <si>
@@ -81,106 +87,106 @@
     <t>Nome (abbrev.)</t>
   </si>
   <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Elenco di valori (separati da virgola)</t>
+  </si>
+  <si>
+    <t>Dim. massima</t>
+  </si>
+  <si>
+    <t>Obbligatorio</t>
+  </si>
+  <si>
+    <t>Valore predefinito</t>
+  </si>
+  <si>
+    <t>Sola lettura</t>
+  </si>
+  <si>
+    <t>Visibile</t>
+  </si>
+  <si>
+    <t>Forza</t>
+  </si>
+  <si>
+    <t>Valore unico</t>
+  </si>
+  <si>
+    <t>Opzioni campo</t>
+  </si>
+  <si>
+    <t>Scheda dati per suggerimento</t>
+  </si>
+  <si>
+    <t>Campo suggerimento</t>
+  </si>
+  <si>
+    <t>Testo aiuto</t>
+  </si>
+  <si>
+    <t>Configurazione Scheda Dati</t>
+  </si>
+  <si>
+    <t>Nome Scheda Dati</t>
+  </si>
+  <si>
+    <t>Descrizione Scheda Dati</t>
+  </si>
+  <si>
+    <t>Ordina scheda per</t>
+  </si>
+  <si>
+    <t>Direzione ordinamento</t>
+  </si>
+  <si>
+    <t>Consenti modifiche</t>
+  </si>
+  <si>
+    <t>Consenti inserimenti</t>
+  </si>
+  <si>
+    <t>Consenti cancellazioni</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Testo</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Sì</t>
+  </si>
+  <si>
+    <t>Maiuscolo</t>
+  </si>
+  <si>
     <t>COD. VOLONTARIO</t>
   </si>
   <si>
+    <t>Data</t>
+  </si>
+  <si>
     <t>COD. ORGANIZZAZIONE</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Testo</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Elenco di valori (separati da virgola)</t>
-  </si>
-  <si>
-    <t>Dim. massima</t>
-  </si>
-  <si>
-    <t>Obbligatorio</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Valore predefinito</t>
-  </si>
-  <si>
-    <t>Sola lettura</t>
-  </si>
-  <si>
-    <t>Visibile</t>
-  </si>
-  <si>
-    <t>Sì</t>
-  </si>
-  <si>
-    <t>Forza</t>
-  </si>
-  <si>
-    <t>Maiuscolo</t>
-  </si>
-  <si>
-    <t>Valore unico</t>
-  </si>
-  <si>
-    <t>Opzioni campo</t>
-  </si>
-  <si>
-    <t>Scheda dati per suggerimento</t>
-  </si>
-  <si>
-    <t>Campo suggerimento</t>
-  </si>
-  <si>
-    <t>Testo aiuto</t>
-  </si>
-  <si>
-    <t>Configurazione Scheda Dati</t>
+    <t>VOLONTARI ATTESI</t>
+  </si>
+  <si>
+    <t>Volontari attesi</t>
+  </si>
+  <si>
+    <t>Crescente</t>
+  </si>
+  <si>
+    <t>RISORSE ATTESE</t>
   </si>
   <si>
     <t>Elenco segnalibri</t>
-  </si>
-  <si>
-    <t>Nome Scheda Dati</t>
-  </si>
-  <si>
-    <t>VOLONTARI ATTESI</t>
-  </si>
-  <si>
-    <t>Descrizione Scheda Dati</t>
-  </si>
-  <si>
-    <t>Volontari attesi</t>
-  </si>
-  <si>
-    <t>Ordina scheda per</t>
-  </si>
-  <si>
-    <t>Direzione ordinamento</t>
-  </si>
-  <si>
-    <t>Crescente</t>
-  </si>
-  <si>
-    <t>Consenti modifiche</t>
-  </si>
-  <si>
-    <t>Consenti inserimenti</t>
-  </si>
-  <si>
-    <t>Consenti cancellazioni</t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>RISORSE ATTESE</t>
   </si>
 </sst>
 </file>
@@ -204,10 +210,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -218,7 +221,7 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,11 +518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,7 +530,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,13 +587,19 @@
       </c>
       <c r="S1" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -599,15 +608,16 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,7 +625,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:22">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -673,10 +683,16 @@
       <c r="T1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -727,18 +743,24 @@
         <v>15</v>
       </c>
       <c r="R2">
+        <v>16</v>
+      </c>
+      <c r="S2">
+        <v>17</v>
+      </c>
+      <c r="T2">
         <v>20</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>21</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -756,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -789,80 +811,92 @@
         <v>15</v>
       </c>
       <c r="R3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="S3" t="s">
         <v>17</v>
       </c>
       <c r="T3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>51</v>
+      </c>
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>26</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -883,134 +917,148 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5"/>
+      <c r="V5"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>255</v>
+      </c>
+      <c r="C6">
+        <v>255</v>
+      </c>
+      <c r="D6">
+        <v>255</v>
+      </c>
+      <c r="E6">
+        <v>255</v>
+      </c>
+      <c r="F6">
+        <v>255</v>
+      </c>
+      <c r="G6">
+        <v>255</v>
+      </c>
+      <c r="H6">
+        <v>255</v>
+      </c>
+      <c r="I6">
+        <v>255</v>
+      </c>
+      <c r="J6">
+        <v>255</v>
+      </c>
+      <c r="K6">
+        <v>255</v>
+      </c>
+      <c r="L6">
+        <v>255</v>
+      </c>
+      <c r="M6">
+        <v>255</v>
+      </c>
+      <c r="N6">
+        <v>255</v>
+      </c>
+      <c r="O6">
+        <v>255</v>
+      </c>
+      <c r="P6">
+        <v>255</v>
+      </c>
+      <c r="Q6">
+        <v>255</v>
+      </c>
+      <c r="R6">
+        <v>255</v>
+      </c>
+      <c r="S6">
+        <v>255</v>
+      </c>
+      <c r="T6">
+        <v>255</v>
+      </c>
+      <c r="U6">
+        <v>255</v>
+      </c>
+      <c r="V6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" t="s">
+        <v>46</v>
+      </c>
+      <c r="V7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" t="s">
         <v>27</v>
-      </c>
-      <c r="B6">
-        <v>255</v>
-      </c>
-      <c r="C6">
-        <v>255</v>
-      </c>
-      <c r="D6">
-        <v>255</v>
-      </c>
-      <c r="E6">
-        <v>255</v>
-      </c>
-      <c r="F6">
-        <v>255</v>
-      </c>
-      <c r="G6">
-        <v>255</v>
-      </c>
-      <c r="H6">
-        <v>255</v>
-      </c>
-      <c r="I6">
-        <v>255</v>
-      </c>
-      <c r="J6">
-        <v>255</v>
-      </c>
-      <c r="K6">
-        <v>255</v>
-      </c>
-      <c r="L6">
-        <v>255</v>
-      </c>
-      <c r="M6">
-        <v>255</v>
-      </c>
-      <c r="N6">
-        <v>255</v>
-      </c>
-      <c r="O6">
-        <v>255</v>
-      </c>
-      <c r="P6">
-        <v>255</v>
-      </c>
-      <c r="Q6">
-        <v>255</v>
-      </c>
-      <c r="R6">
-        <v>255</v>
-      </c>
-      <c r="S6">
-        <v>255</v>
-      </c>
-      <c r="T6">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" t="s">
-        <v>30</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -1031,244 +1079,266 @@
       <c r="R8"/>
       <c r="S8"/>
       <c r="T8"/>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8"/>
+      <c r="V8"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>46</v>
+      </c>
+      <c r="R9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" t="s">
+        <v>46</v>
+      </c>
+      <c r="T9" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="L10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="N10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="O10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="P10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="Q10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="R10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="S10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="T10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>47</v>
+      </c>
+      <c r="U10" t="s">
+        <v>47</v>
+      </c>
+      <c r="V10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="I11"/>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="K11"/>
-      <c r="L11" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" t="s">
-        <v>29</v>
-      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
       <c r="O11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
+        <v>46</v>
+      </c>
+      <c r="P11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R11" t="s">
+        <v>46</v>
+      </c>
       <c r="S11"/>
-      <c r="T11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="O12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="P12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="Q12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="R12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="S12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="T12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>46</v>
+      </c>
+      <c r="U12" t="s">
+        <v>46</v>
+      </c>
+      <c r="V12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -1289,10 +1359,12 @@
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13"/>
+      <c r="V13"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -1313,10 +1385,12 @@
       <c r="R14"/>
       <c r="S14"/>
       <c r="T14"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14"/>
+      <c r="V14"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -1337,10 +1411,12 @@
       <c r="R15"/>
       <c r="S15"/>
       <c r="T15"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15"/>
+      <c r="V15"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -1361,84 +1437,86 @@
       <c r="R16"/>
       <c r="S16"/>
       <c r="T16"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16"/>
+      <c r="V16"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -1447,5 +1525,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>